<commit_message>
Updated stats to include ROTH
</commit_message>
<xml_diff>
--- a/data/historic-performance.xlsx
+++ b/data/historic-performance.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15240" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="Both" sheetId="1" r:id="rId1"/>
+    <sheet name="Roth" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="18">
   <si>
     <t>2013 (TBC…)</t>
   </si>
@@ -44,6 +45,36 @@
   <si>
     <t>Jarvis w/o Comm Returns</t>
   </si>
+  <si>
+    <t>w/commissions</t>
+  </si>
+  <si>
+    <t>w/o commissions</t>
+  </si>
+  <si>
+    <t>S&amp;P 2010 YTD</t>
+  </si>
+  <si>
+    <t>Jarvis Fund (w/ E*Trade Commissions)</t>
+  </si>
+  <si>
+    <t>Jarvis Fund (w/o E*Trade Commissions)</t>
+  </si>
+  <si>
+    <t>Jarvis Fund (w/ JF fees)</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>Management Fee</t>
+  </si>
+  <si>
+    <t>Performance Fee</t>
+  </si>
+  <si>
+    <t>w JF fees</t>
+  </si>
 </sst>
 </file>
 
@@ -51,7 +82,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -115,7 +146,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -222,8 +253,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="101">
+  <cellStyleXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -325,8 +365,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -349,37 +421,47 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -389,12 +471,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="101">
+  <cellStyles count="133">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -445,6 +567,22 @@
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -494,6 +632,22 @@
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -826,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T259"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T99" sqref="T99"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -842,30 +996,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="27" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="28"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="32"/>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="22" t="s">
@@ -893,7 +1047,7 @@
         <v>7</v>
       </c>
       <c r="K2" s="22"/>
-      <c r="L2" s="30">
+      <c r="L2" s="29">
         <f>(L4*N4*P4*R4*T4)-1</f>
         <v>0.42143857852697053</v>
       </c>
@@ -1128,46 +1282,46 @@
       </c>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="27">
+      <c r="A6" s="31">
         <v>2009</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="27">
+      <c r="B6" s="32"/>
+      <c r="C6" s="31">
         <v>2010</v>
       </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="27">
+      <c r="D6" s="32"/>
+      <c r="E6" s="31">
         <v>2011</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="27">
+      <c r="F6" s="32"/>
+      <c r="G6" s="31">
         <v>2012</v>
       </c>
-      <c r="H6" s="28"/>
-      <c r="I6" s="27" t="s">
+      <c r="H6" s="32"/>
+      <c r="I6" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="28"/>
-      <c r="K6" s="27">
+      <c r="J6" s="32"/>
+      <c r="K6" s="31">
         <v>2009</v>
       </c>
-      <c r="L6" s="28"/>
-      <c r="M6" s="27">
+      <c r="L6" s="32"/>
+      <c r="M6" s="31">
         <v>2010</v>
       </c>
-      <c r="N6" s="28"/>
-      <c r="O6" s="27">
+      <c r="N6" s="32"/>
+      <c r="O6" s="31">
         <v>2011</v>
       </c>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="27">
+      <c r="P6" s="32"/>
+      <c r="Q6" s="31">
         <v>2012</v>
       </c>
-      <c r="R6" s="28"/>
-      <c r="S6" s="27" t="s">
+      <c r="R6" s="32"/>
+      <c r="S6" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="T6" s="28"/>
+      <c r="T6" s="32"/>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="7">
@@ -1227,14 +1381,14 @@
       <c r="Q7" s="14">
         <v>40909</v>
       </c>
-      <c r="R7" s="31">
+      <c r="R7" s="30">
         <f>-1*P66</f>
         <v>10003.056399999999</v>
       </c>
       <c r="S7" s="14">
         <v>41275</v>
       </c>
-      <c r="T7" s="31">
+      <c r="T7" s="30">
         <f>-1*R63</f>
         <v>20924.761400000003</v>
       </c>
@@ -6205,4 +6359,1981 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="38">
+        <f>D7</f>
+        <v>0.69171811411367878</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="38">
+        <f>B7</f>
+        <v>0.83448085975058972</v>
+      </c>
+      <c r="L2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2">
+        <f>XIRR(M3:M4,L3:L4)</f>
+        <v>8.2821670174598711E-2</v>
+      </c>
+      <c r="T2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2">
+        <f>XIRR(U3:U4,T3:T4)</f>
+        <v>8.2821670174598711E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="38">
+        <f>J7</f>
+        <v>0.90747174980552847</v>
+      </c>
+      <c r="L3" s="1">
+        <v>40274</v>
+      </c>
+      <c r="M3">
+        <v>1186.01</v>
+      </c>
+      <c r="T3" s="1">
+        <v>40274</v>
+      </c>
+      <c r="U3">
+        <v>1186.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="L4" s="37">
+        <v>40543</v>
+      </c>
+      <c r="M4">
+        <v>-1257.6400000000001</v>
+      </c>
+      <c r="T4" s="37">
+        <v>40543</v>
+      </c>
+      <c r="U4">
+        <v>-1257.6400000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="B6" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="S6" s="33"/>
+      <c r="T6" s="33"/>
+      <c r="U6" s="33"/>
+      <c r="V6" s="33"/>
+      <c r="W6" s="33"/>
+      <c r="X6" s="33"/>
+      <c r="Y6" s="32"/>
+    </row>
+    <row r="7" spans="1:25">
+      <c r="B7" s="24">
+        <f>(C9*E9*G9*I9)-1</f>
+        <v>0.83448085975058972</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="26">
+        <f>(B9*D9*F9*H9)-1</f>
+        <v>0.69171811411367878</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="J7" s="24">
+        <f>(K9*M9*O9*Q9)-1</f>
+        <v>0.90747174980552847</v>
+      </c>
+      <c r="K7" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="26">
+        <f>(J9*L9*N9*P9)-1</f>
+        <v>0.69171811411367878</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="24">
+        <f>((S9*U9*W9*Y9)-1)*0.9</f>
+        <v>0.73231143106249885</v>
+      </c>
+      <c r="S7" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="T7" s="26">
+        <f>(R9*T9*V9*X9)-1</f>
+        <v>0.69171811411367878</v>
+      </c>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+    </row>
+    <row r="8" spans="1:25">
+      <c r="B8" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="M8" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="O8" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q8" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="R8" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="S8" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="T8" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="U8" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="V8" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="W8" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="X8" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y8" s="28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="16">
+        <f>1+B10</f>
+        <v>1.0828216701745987</v>
+      </c>
+      <c r="C9" s="17">
+        <f>1+C10</f>
+        <v>1.4991680085659027</v>
+      </c>
+      <c r="D9" s="16">
+        <f>1+D10</f>
+        <v>1.0210999999999999</v>
+      </c>
+      <c r="E9" s="17">
+        <f>1+E10</f>
+        <v>0.61277180537581444</v>
+      </c>
+      <c r="F9" s="16">
+        <f>1+F10</f>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="G9" s="17">
+        <f>1+G10</f>
+        <v>1.3741180837154388</v>
+      </c>
+      <c r="H9" s="16">
+        <f>1+H10</f>
+        <v>1.319</v>
+      </c>
+      <c r="I9" s="17">
+        <f>1+I10</f>
+        <v>1.4532490551471708</v>
+      </c>
+      <c r="J9" s="16">
+        <f>1+J10</f>
+        <v>1.0828216701745987</v>
+      </c>
+      <c r="K9" s="17">
+        <f>1+K10</f>
+        <v>1.5332716047763824</v>
+      </c>
+      <c r="L9" s="16">
+        <f>1+L10</f>
+        <v>1.0210999999999999</v>
+      </c>
+      <c r="M9" s="17">
+        <f>1+M10</f>
+        <v>0.62397755160927759</v>
+      </c>
+      <c r="N9" s="16">
+        <f>1+N10</f>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="O9" s="17">
+        <f>1+O10</f>
+        <v>1.3741329729557039</v>
+      </c>
+      <c r="P9" s="16">
+        <f>1+P10</f>
+        <v>1.319</v>
+      </c>
+      <c r="Q9" s="17">
+        <f>1+Q10</f>
+        <v>1.450912743806839</v>
+      </c>
+      <c r="R9" s="16">
+        <f>1+R10</f>
+        <v>1.0828216701745987</v>
+      </c>
+      <c r="S9" s="17">
+        <f>1+S10</f>
+        <v>1.5061375796794891</v>
+      </c>
+      <c r="T9" s="16">
+        <f>1+T10</f>
+        <v>1.0210999999999999</v>
+      </c>
+      <c r="U9" s="17">
+        <f>1+U10</f>
+        <v>0.61207630857825268</v>
+      </c>
+      <c r="V9" s="16">
+        <f>1+V10</f>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="W9" s="17">
+        <f>1+W10</f>
+        <v>1.3651962578296661</v>
+      </c>
+      <c r="X9" s="16">
+        <f>1+X10</f>
+        <v>1.319</v>
+      </c>
+      <c r="Y9" s="17">
+        <f>1+Y10</f>
+        <v>1.4411036193370821</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25">
+      <c r="B10" s="20">
+        <f>M2</f>
+        <v>8.2821670174598711E-2</v>
+      </c>
+      <c r="C10" s="21">
+        <f>XIRR(C14:C21,B14:B21)</f>
+        <v>0.49916800856590271</v>
+      </c>
+      <c r="D10" s="20">
+        <v>2.1100000000000001E-2</v>
+      </c>
+      <c r="E10" s="21">
+        <f>XIRR(E14:E20,D14:D20)</f>
+        <v>-0.38722819462418551</v>
+      </c>
+      <c r="F10" s="20">
+        <v>0.16</v>
+      </c>
+      <c r="G10" s="21">
+        <f>XIRR(G14:G22,F14:F22)</f>
+        <v>0.37411808371543886</v>
+      </c>
+      <c r="H10" s="20">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="I10" s="21">
+        <f>XIRR(I14:I854,H14:H854)</f>
+        <v>0.45324905514717095</v>
+      </c>
+      <c r="J10" s="20">
+        <f>M2</f>
+        <v>8.2821670174598711E-2</v>
+      </c>
+      <c r="K10" s="21">
+        <f>XIRR(K14:K21,J14:J21)</f>
+        <v>0.53327160477638247</v>
+      </c>
+      <c r="L10" s="20">
+        <v>2.1100000000000001E-2</v>
+      </c>
+      <c r="M10" s="21">
+        <f>XIRR(M14:M20,L14:L20)</f>
+        <v>-0.37602244839072235</v>
+      </c>
+      <c r="N10" s="20">
+        <v>0.16</v>
+      </c>
+      <c r="O10" s="21">
+        <f>XIRR(O14:O22,N14:N22)</f>
+        <v>0.3741329729557038</v>
+      </c>
+      <c r="P10" s="20">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="Q10" s="21">
+        <f>XIRR(Q14:Q854,P14:P854)</f>
+        <v>0.45091274380683899</v>
+      </c>
+      <c r="R10" s="20">
+        <f>U2</f>
+        <v>8.2821670174598711E-2</v>
+      </c>
+      <c r="S10" s="21">
+        <f>XIRR(S14:S21,R14:R21)</f>
+        <v>0.50613757967948914</v>
+      </c>
+      <c r="T10" s="20">
+        <v>2.1100000000000001E-2</v>
+      </c>
+      <c r="U10" s="21">
+        <f>XIRR(U14:U20,T14:T20)</f>
+        <v>-0.38792369142174732</v>
+      </c>
+      <c r="V10" s="20">
+        <v>0.16</v>
+      </c>
+      <c r="W10" s="21">
+        <f>XIRR(W14:W22,V14:V22)</f>
+        <v>0.36519625782966614</v>
+      </c>
+      <c r="X10" s="20">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="Y10" s="21">
+        <f>XIRR(Y14:Y854,X14:X854)</f>
+        <v>0.44110361933708198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="40"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="42"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="42"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="42"/>
+      <c r="S11" s="41"/>
+      <c r="T11" s="42"/>
+      <c r="U11" s="41"/>
+      <c r="V11" s="42"/>
+      <c r="W11" s="41"/>
+      <c r="X11" s="42"/>
+      <c r="Y11" s="43"/>
+    </row>
+    <row r="12" spans="1:25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="46">
+        <f>K21*0.01</f>
+        <v>-39.704000000000001</v>
+      </c>
+      <c r="L12" s="45"/>
+      <c r="M12" s="47">
+        <f>M20*0.01</f>
+        <v>-36.961799999999997</v>
+      </c>
+      <c r="N12" s="48"/>
+      <c r="O12" s="47">
+        <f>0.01*O22</f>
+        <v>-70.3215</v>
+      </c>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="49">
+        <f>0.01*Q60</f>
+        <v>-147.24959999999999</v>
+      </c>
+      <c r="R12" s="45"/>
+      <c r="S12" s="46">
+        <f>S21*0.01</f>
+        <v>-39.306959999999997</v>
+      </c>
+      <c r="T12" s="45"/>
+      <c r="U12" s="47">
+        <f>U20*0.01</f>
+        <v>-36.195141999999997</v>
+      </c>
+      <c r="V12" s="48"/>
+      <c r="W12" s="47">
+        <f>0.01*W22</f>
+        <v>-68.851627000000008</v>
+      </c>
+      <c r="X12" s="48"/>
+      <c r="Y12" s="49">
+        <f>0.01*Y60</f>
+        <v>-144.307231</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="B13" s="31">
+        <v>2010</v>
+      </c>
+      <c r="C13" s="32"/>
+      <c r="D13" s="31">
+        <v>2011</v>
+      </c>
+      <c r="E13" s="32"/>
+      <c r="F13" s="31">
+        <v>2012</v>
+      </c>
+      <c r="G13" s="32"/>
+      <c r="H13" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" s="32"/>
+      <c r="J13" s="31">
+        <v>2010</v>
+      </c>
+      <c r="K13" s="32"/>
+      <c r="L13" s="31">
+        <v>2011</v>
+      </c>
+      <c r="M13" s="32"/>
+      <c r="N13" s="31">
+        <v>2012</v>
+      </c>
+      <c r="O13" s="32"/>
+      <c r="P13" s="31">
+        <v>2013</v>
+      </c>
+      <c r="Q13" s="32"/>
+      <c r="R13" s="31">
+        <v>2010</v>
+      </c>
+      <c r="S13" s="32"/>
+      <c r="T13" s="31">
+        <v>2011</v>
+      </c>
+      <c r="U13" s="32"/>
+      <c r="V13" s="31">
+        <v>2012</v>
+      </c>
+      <c r="W13" s="32"/>
+      <c r="X13" s="31">
+        <v>2013</v>
+      </c>
+      <c r="Y13" s="32"/>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="B14" s="1">
+        <v>40274</v>
+      </c>
+      <c r="C14">
+        <v>300</v>
+      </c>
+      <c r="D14" s="34">
+        <v>40544</v>
+      </c>
+      <c r="E14" s="35">
+        <f>-C21</f>
+        <v>3920.45</v>
+      </c>
+      <c r="F14" s="34">
+        <v>40909</v>
+      </c>
+      <c r="G14" s="36">
+        <f>-E20</f>
+        <v>3616.26</v>
+      </c>
+      <c r="H14" s="34">
+        <v>41275</v>
+      </c>
+      <c r="I14" s="36">
+        <f>-G22</f>
+        <v>6922.26</v>
+      </c>
+      <c r="J14" s="1">
+        <v>40274</v>
+      </c>
+      <c r="K14">
+        <v>300</v>
+      </c>
+      <c r="L14" s="34">
+        <v>40544</v>
+      </c>
+      <c r="M14" s="35">
+        <f>-K21</f>
+        <v>3970.3999999999996</v>
+      </c>
+      <c r="N14" s="34">
+        <v>40909</v>
+      </c>
+      <c r="O14" s="36">
+        <f>-M20</f>
+        <v>3696.18</v>
+      </c>
+      <c r="P14" s="34">
+        <v>41275</v>
+      </c>
+      <c r="Q14" s="36">
+        <f>-O22</f>
+        <v>7032.1500000000005</v>
+      </c>
+      <c r="R14" s="1">
+        <v>40274</v>
+      </c>
+      <c r="S14">
+        <v>300</v>
+      </c>
+      <c r="T14" s="34">
+        <v>40544</v>
+      </c>
+      <c r="U14" s="35">
+        <f>-S21</f>
+        <v>3930.6959999999995</v>
+      </c>
+      <c r="V14" s="34">
+        <v>40909</v>
+      </c>
+      <c r="W14" s="36">
+        <f>-U20</f>
+        <v>3619.5141999999996</v>
+      </c>
+      <c r="X14" s="34">
+        <v>41275</v>
+      </c>
+      <c r="Y14" s="36">
+        <f>-W22</f>
+        <v>6885.1627000000008</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="B15" s="1">
+        <v>40301</v>
+      </c>
+      <c r="C15">
+        <v>500</v>
+      </c>
+      <c r="D15" s="1">
+        <v>40774</v>
+      </c>
+      <c r="E15">
+        <v>400</v>
+      </c>
+      <c r="F15" s="1">
+        <v>40939</v>
+      </c>
+      <c r="G15">
+        <v>150</v>
+      </c>
+      <c r="H15" s="1">
+        <v>41281</v>
+      </c>
+      <c r="I15">
+        <v>50</v>
+      </c>
+      <c r="J15" s="1">
+        <v>40301</v>
+      </c>
+      <c r="K15">
+        <v>500</v>
+      </c>
+      <c r="L15" s="1">
+        <v>40774</v>
+      </c>
+      <c r="M15">
+        <v>400</v>
+      </c>
+      <c r="N15" s="1">
+        <v>40939</v>
+      </c>
+      <c r="O15">
+        <v>150</v>
+      </c>
+      <c r="P15" s="1">
+        <v>41281</v>
+      </c>
+      <c r="Q15">
+        <v>50</v>
+      </c>
+      <c r="R15" s="1">
+        <v>40301</v>
+      </c>
+      <c r="S15">
+        <v>500</v>
+      </c>
+      <c r="T15" s="1">
+        <v>40774</v>
+      </c>
+      <c r="U15">
+        <v>400</v>
+      </c>
+      <c r="V15" s="1">
+        <v>40939</v>
+      </c>
+      <c r="W15">
+        <v>150</v>
+      </c>
+      <c r="X15" s="1">
+        <v>41281</v>
+      </c>
+      <c r="Y15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25">
+      <c r="B16" s="1">
+        <v>40338</v>
+      </c>
+      <c r="C16">
+        <v>800</v>
+      </c>
+      <c r="D16" s="1">
+        <v>40841</v>
+      </c>
+      <c r="E16">
+        <v>300</v>
+      </c>
+      <c r="F16" s="1">
+        <v>40946</v>
+      </c>
+      <c r="G16">
+        <v>150</v>
+      </c>
+      <c r="H16" s="1">
+        <v>41288</v>
+      </c>
+      <c r="I16">
+        <v>50</v>
+      </c>
+      <c r="J16" s="1">
+        <v>40338</v>
+      </c>
+      <c r="K16">
+        <v>800</v>
+      </c>
+      <c r="L16" s="1">
+        <v>40841</v>
+      </c>
+      <c r="M16">
+        <v>300</v>
+      </c>
+      <c r="N16" s="1">
+        <v>40946</v>
+      </c>
+      <c r="O16">
+        <v>150</v>
+      </c>
+      <c r="P16" s="1">
+        <v>41288</v>
+      </c>
+      <c r="Q16">
+        <v>50</v>
+      </c>
+      <c r="R16" s="1">
+        <v>40338</v>
+      </c>
+      <c r="S16">
+        <v>800</v>
+      </c>
+      <c r="T16" s="1">
+        <v>40841</v>
+      </c>
+      <c r="U16">
+        <v>300</v>
+      </c>
+      <c r="V16" s="1">
+        <v>40946</v>
+      </c>
+      <c r="W16">
+        <v>150</v>
+      </c>
+      <c r="X16" s="1">
+        <v>41288</v>
+      </c>
+      <c r="Y16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="2:25">
+      <c r="B17" s="1">
+        <v>40346</v>
+      </c>
+      <c r="C17">
+        <v>500</v>
+      </c>
+      <c r="D17" s="1">
+        <v>40843</v>
+      </c>
+      <c r="E17">
+        <v>300</v>
+      </c>
+      <c r="F17" s="1">
+        <v>40961</v>
+      </c>
+      <c r="G17">
+        <v>150</v>
+      </c>
+      <c r="H17" s="1">
+        <v>41296</v>
+      </c>
+      <c r="I17">
+        <v>50</v>
+      </c>
+      <c r="J17" s="1">
+        <v>40346</v>
+      </c>
+      <c r="K17">
+        <v>500</v>
+      </c>
+      <c r="L17" s="1">
+        <v>40843</v>
+      </c>
+      <c r="M17">
+        <v>300</v>
+      </c>
+      <c r="N17" s="1">
+        <v>40961</v>
+      </c>
+      <c r="O17">
+        <v>150</v>
+      </c>
+      <c r="P17" s="1">
+        <v>41296</v>
+      </c>
+      <c r="Q17">
+        <v>50</v>
+      </c>
+      <c r="R17" s="1">
+        <v>40346</v>
+      </c>
+      <c r="S17">
+        <v>500</v>
+      </c>
+      <c r="T17" s="1">
+        <v>40843</v>
+      </c>
+      <c r="U17">
+        <v>300</v>
+      </c>
+      <c r="V17" s="1">
+        <v>40961</v>
+      </c>
+      <c r="W17">
+        <v>150</v>
+      </c>
+      <c r="X17" s="1">
+        <v>41296</v>
+      </c>
+      <c r="Y17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:25">
+      <c r="B18" s="1">
+        <v>40351</v>
+      </c>
+      <c r="C18">
+        <v>800</v>
+      </c>
+      <c r="D18" s="1">
+        <v>40849</v>
+      </c>
+      <c r="E18">
+        <v>150</v>
+      </c>
+      <c r="F18" s="1">
+        <v>40967</v>
+      </c>
+      <c r="G18">
+        <v>150</v>
+      </c>
+      <c r="H18" s="1">
+        <v>41302</v>
+      </c>
+      <c r="I18">
+        <v>50</v>
+      </c>
+      <c r="J18" s="1">
+        <v>40351</v>
+      </c>
+      <c r="K18">
+        <v>800</v>
+      </c>
+      <c r="L18" s="1">
+        <v>40849</v>
+      </c>
+      <c r="M18">
+        <v>150</v>
+      </c>
+      <c r="N18" s="1">
+        <v>40967</v>
+      </c>
+      <c r="O18">
+        <v>150</v>
+      </c>
+      <c r="P18" s="1">
+        <v>41302</v>
+      </c>
+      <c r="Q18">
+        <v>50</v>
+      </c>
+      <c r="R18" s="1">
+        <v>40351</v>
+      </c>
+      <c r="S18">
+        <v>800</v>
+      </c>
+      <c r="T18" s="1">
+        <v>40849</v>
+      </c>
+      <c r="U18">
+        <v>150</v>
+      </c>
+      <c r="V18" s="1">
+        <v>40967</v>
+      </c>
+      <c r="W18">
+        <v>150</v>
+      </c>
+      <c r="X18" s="1">
+        <v>41302</v>
+      </c>
+      <c r="Y18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="2:25">
+      <c r="B19" s="1">
+        <v>40436</v>
+      </c>
+      <c r="C19">
+        <v>75</v>
+      </c>
+      <c r="D19" s="1">
+        <v>40865</v>
+      </c>
+      <c r="E19">
+        <v>200</v>
+      </c>
+      <c r="F19" s="1">
+        <v>40974</v>
+      </c>
+      <c r="G19">
+        <v>150</v>
+      </c>
+      <c r="H19" s="1">
+        <v>41309</v>
+      </c>
+      <c r="I19">
+        <v>50</v>
+      </c>
+      <c r="J19" s="1">
+        <v>40436</v>
+      </c>
+      <c r="K19">
+        <v>75</v>
+      </c>
+      <c r="L19" s="1">
+        <v>40865</v>
+      </c>
+      <c r="M19">
+        <v>200</v>
+      </c>
+      <c r="N19" s="1">
+        <v>40974</v>
+      </c>
+      <c r="O19">
+        <v>150</v>
+      </c>
+      <c r="P19" s="1">
+        <v>41309</v>
+      </c>
+      <c r="Q19">
+        <v>50</v>
+      </c>
+      <c r="R19" s="1">
+        <v>40436</v>
+      </c>
+      <c r="S19">
+        <v>75</v>
+      </c>
+      <c r="T19" s="1">
+        <v>40865</v>
+      </c>
+      <c r="U19">
+        <v>200</v>
+      </c>
+      <c r="V19" s="1">
+        <v>40974</v>
+      </c>
+      <c r="W19">
+        <v>150</v>
+      </c>
+      <c r="X19" s="1">
+        <v>41309</v>
+      </c>
+      <c r="Y19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="2:25">
+      <c r="B20" s="1">
+        <v>40477</v>
+      </c>
+      <c r="C20">
+        <v>150</v>
+      </c>
+      <c r="D20" s="1">
+        <v>40908</v>
+      </c>
+      <c r="E20">
+        <v>-3616.26</v>
+      </c>
+      <c r="F20" s="1">
+        <v>41024</v>
+      </c>
+      <c r="G20">
+        <v>300</v>
+      </c>
+      <c r="H20" s="1">
+        <v>41316</v>
+      </c>
+      <c r="I20">
+        <v>50</v>
+      </c>
+      <c r="J20" s="1">
+        <v>40477</v>
+      </c>
+      <c r="K20">
+        <v>150</v>
+      </c>
+      <c r="L20" s="1">
+        <v>40908</v>
+      </c>
+      <c r="M20">
+        <f>E20-49.95-29.97</f>
+        <v>-3696.18</v>
+      </c>
+      <c r="N20" s="1">
+        <v>41024</v>
+      </c>
+      <c r="O20">
+        <v>300</v>
+      </c>
+      <c r="P20" s="1">
+        <v>41316</v>
+      </c>
+      <c r="Q20">
+        <v>50</v>
+      </c>
+      <c r="R20" s="1">
+        <v>40477</v>
+      </c>
+      <c r="S20">
+        <v>150</v>
+      </c>
+      <c r="T20" s="1">
+        <v>40908</v>
+      </c>
+      <c r="U20" s="50">
+        <f>M20-K12-M12</f>
+        <v>-3619.5141999999996</v>
+      </c>
+      <c r="V20" s="1">
+        <v>41024</v>
+      </c>
+      <c r="W20">
+        <v>300</v>
+      </c>
+      <c r="X20" s="1">
+        <v>41316</v>
+      </c>
+      <c r="Y20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="2:25">
+      <c r="B21" s="1">
+        <v>40543</v>
+      </c>
+      <c r="C21">
+        <v>-3920.45</v>
+      </c>
+      <c r="F21" s="1">
+        <v>41080</v>
+      </c>
+      <c r="G21">
+        <v>500</v>
+      </c>
+      <c r="H21" s="1">
+        <v>41324</v>
+      </c>
+      <c r="I21">
+        <v>50</v>
+      </c>
+      <c r="J21" s="1">
+        <v>40543</v>
+      </c>
+      <c r="K21">
+        <f>C21-49.95</f>
+        <v>-3970.3999999999996</v>
+      </c>
+      <c r="N21" s="1">
+        <v>41080</v>
+      </c>
+      <c r="O21">
+        <v>500</v>
+      </c>
+      <c r="P21" s="1">
+        <v>41324</v>
+      </c>
+      <c r="Q21">
+        <v>50</v>
+      </c>
+      <c r="R21" s="1">
+        <v>40543</v>
+      </c>
+      <c r="S21" s="51">
+        <f>K21-K12</f>
+        <v>-3930.6959999999995</v>
+      </c>
+      <c r="V21" s="1">
+        <v>41080</v>
+      </c>
+      <c r="W21">
+        <v>500</v>
+      </c>
+      <c r="X21" s="1">
+        <v>41324</v>
+      </c>
+      <c r="Y21">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="2:25">
+      <c r="F22" s="1">
+        <v>41274</v>
+      </c>
+      <c r="G22">
+        <v>-6922.26</v>
+      </c>
+      <c r="H22" s="1">
+        <v>41330</v>
+      </c>
+      <c r="I22">
+        <v>50</v>
+      </c>
+      <c r="N22" s="1">
+        <v>41274</v>
+      </c>
+      <c r="O22">
+        <f>G22-49.95-29.97-29.97</f>
+        <v>-7032.1500000000005</v>
+      </c>
+      <c r="P22" s="1">
+        <v>41330</v>
+      </c>
+      <c r="Q22">
+        <v>50</v>
+      </c>
+      <c r="V22" s="1">
+        <v>41274</v>
+      </c>
+      <c r="W22" s="50">
+        <f>O22-SUM(K12:O12)</f>
+        <v>-6885.1627000000008</v>
+      </c>
+      <c r="X22" s="1">
+        <v>41330</v>
+      </c>
+      <c r="Y22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="2:25">
+      <c r="H23" s="1">
+        <v>41337</v>
+      </c>
+      <c r="I23">
+        <v>50</v>
+      </c>
+      <c r="P23" s="1">
+        <v>41337</v>
+      </c>
+      <c r="Q23">
+        <v>50</v>
+      </c>
+      <c r="X23" s="1">
+        <v>41337</v>
+      </c>
+      <c r="Y23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="2:25">
+      <c r="H24" s="1">
+        <v>41344</v>
+      </c>
+      <c r="I24">
+        <v>50</v>
+      </c>
+      <c r="P24" s="1">
+        <v>41344</v>
+      </c>
+      <c r="Q24">
+        <v>50</v>
+      </c>
+      <c r="X24" s="1">
+        <v>41344</v>
+      </c>
+      <c r="Y24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="2:25">
+      <c r="H25" s="1">
+        <v>41351</v>
+      </c>
+      <c r="I25">
+        <v>50</v>
+      </c>
+      <c r="P25" s="1">
+        <v>41351</v>
+      </c>
+      <c r="Q25">
+        <v>50</v>
+      </c>
+      <c r="X25" s="1">
+        <v>41351</v>
+      </c>
+      <c r="Y25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="2:25">
+      <c r="H26" s="1">
+        <v>41358</v>
+      </c>
+      <c r="I26">
+        <v>50</v>
+      </c>
+      <c r="P26" s="1">
+        <v>41358</v>
+      </c>
+      <c r="Q26">
+        <v>50</v>
+      </c>
+      <c r="X26" s="1">
+        <v>41358</v>
+      </c>
+      <c r="Y26">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="2:25">
+      <c r="H27" s="1">
+        <v>41365</v>
+      </c>
+      <c r="I27">
+        <v>50</v>
+      </c>
+      <c r="P27" s="1">
+        <v>41365</v>
+      </c>
+      <c r="Q27">
+        <v>50</v>
+      </c>
+      <c r="X27" s="1">
+        <v>41365</v>
+      </c>
+      <c r="Y27">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="2:25">
+      <c r="H28" s="1">
+        <v>41372</v>
+      </c>
+      <c r="I28">
+        <v>50</v>
+      </c>
+      <c r="P28" s="1">
+        <v>41372</v>
+      </c>
+      <c r="Q28">
+        <v>50</v>
+      </c>
+      <c r="X28" s="1">
+        <v>41372</v>
+      </c>
+      <c r="Y28">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="2:25">
+      <c r="H29" s="1">
+        <v>41379</v>
+      </c>
+      <c r="I29">
+        <v>50</v>
+      </c>
+      <c r="P29" s="1">
+        <v>41379</v>
+      </c>
+      <c r="Q29">
+        <v>50</v>
+      </c>
+      <c r="X29" s="1">
+        <v>41379</v>
+      </c>
+      <c r="Y29">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="2:25">
+      <c r="H30" s="1">
+        <v>41400</v>
+      </c>
+      <c r="I30">
+        <v>100</v>
+      </c>
+      <c r="P30" s="1">
+        <v>41400</v>
+      </c>
+      <c r="Q30">
+        <v>100</v>
+      </c>
+      <c r="X30" s="1">
+        <v>41400</v>
+      </c>
+      <c r="Y30">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="2:25">
+      <c r="H31" s="1">
+        <v>41407</v>
+      </c>
+      <c r="I31">
+        <v>100</v>
+      </c>
+      <c r="P31" s="1">
+        <v>41407</v>
+      </c>
+      <c r="Q31">
+        <v>100</v>
+      </c>
+      <c r="X31" s="1">
+        <v>41407</v>
+      </c>
+      <c r="Y31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="2:25">
+      <c r="H32" s="1">
+        <v>41414</v>
+      </c>
+      <c r="I32">
+        <v>100</v>
+      </c>
+      <c r="P32" s="1">
+        <v>41414</v>
+      </c>
+      <c r="Q32">
+        <v>100</v>
+      </c>
+      <c r="X32" s="1">
+        <v>41414</v>
+      </c>
+      <c r="Y32">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="8:25">
+      <c r="H33" s="1">
+        <v>41422</v>
+      </c>
+      <c r="I33">
+        <v>100</v>
+      </c>
+      <c r="P33" s="1">
+        <v>41422</v>
+      </c>
+      <c r="Q33">
+        <v>100</v>
+      </c>
+      <c r="X33" s="1">
+        <v>41422</v>
+      </c>
+      <c r="Y33">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="8:25">
+      <c r="H34" s="1">
+        <v>41428</v>
+      </c>
+      <c r="I34">
+        <v>100</v>
+      </c>
+      <c r="P34" s="1">
+        <v>41428</v>
+      </c>
+      <c r="Q34">
+        <v>100</v>
+      </c>
+      <c r="X34" s="1">
+        <v>41428</v>
+      </c>
+      <c r="Y34">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="8:25">
+      <c r="H35" s="1">
+        <v>41435</v>
+      </c>
+      <c r="I35">
+        <v>100</v>
+      </c>
+      <c r="P35" s="1">
+        <v>41435</v>
+      </c>
+      <c r="Q35">
+        <v>100</v>
+      </c>
+      <c r="X35" s="1">
+        <v>41435</v>
+      </c>
+      <c r="Y35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="8:25">
+      <c r="H36" s="1">
+        <v>41442</v>
+      </c>
+      <c r="I36">
+        <v>100</v>
+      </c>
+      <c r="P36" s="1">
+        <v>41442</v>
+      </c>
+      <c r="Q36">
+        <v>100</v>
+      </c>
+      <c r="X36" s="1">
+        <v>41442</v>
+      </c>
+      <c r="Y36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="8:25">
+      <c r="H37" s="1">
+        <v>41449</v>
+      </c>
+      <c r="I37">
+        <v>100</v>
+      </c>
+      <c r="P37" s="1">
+        <v>41449</v>
+      </c>
+      <c r="Q37">
+        <v>100</v>
+      </c>
+      <c r="X37" s="1">
+        <v>41449</v>
+      </c>
+      <c r="Y37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="8:25">
+      <c r="H38" s="1">
+        <v>41456</v>
+      </c>
+      <c r="I38">
+        <v>100</v>
+      </c>
+      <c r="P38" s="1">
+        <v>41456</v>
+      </c>
+      <c r="Q38">
+        <v>100</v>
+      </c>
+      <c r="X38" s="1">
+        <v>41456</v>
+      </c>
+      <c r="Y38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="8:25">
+      <c r="H39" s="1">
+        <v>41463</v>
+      </c>
+      <c r="I39">
+        <v>100</v>
+      </c>
+      <c r="P39" s="1">
+        <v>41463</v>
+      </c>
+      <c r="Q39">
+        <v>100</v>
+      </c>
+      <c r="X39" s="1">
+        <v>41463</v>
+      </c>
+      <c r="Y39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="8:25">
+      <c r="H40" s="1">
+        <v>41470</v>
+      </c>
+      <c r="I40">
+        <v>100</v>
+      </c>
+      <c r="P40" s="1">
+        <v>41470</v>
+      </c>
+      <c r="Q40">
+        <v>100</v>
+      </c>
+      <c r="X40" s="1">
+        <v>41470</v>
+      </c>
+      <c r="Y40">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="8:25">
+      <c r="H41" s="1">
+        <v>41477</v>
+      </c>
+      <c r="I41">
+        <v>100</v>
+      </c>
+      <c r="P41" s="1">
+        <v>41477</v>
+      </c>
+      <c r="Q41">
+        <v>100</v>
+      </c>
+      <c r="X41" s="1">
+        <v>41477</v>
+      </c>
+      <c r="Y41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="8:25">
+      <c r="H42" s="1">
+        <v>41498</v>
+      </c>
+      <c r="I42">
+        <v>100</v>
+      </c>
+      <c r="P42" s="1">
+        <v>41498</v>
+      </c>
+      <c r="Q42">
+        <v>100</v>
+      </c>
+      <c r="X42" s="1">
+        <v>41498</v>
+      </c>
+      <c r="Y42">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="8:25">
+      <c r="H43" s="1">
+        <v>41505</v>
+      </c>
+      <c r="I43">
+        <v>100</v>
+      </c>
+      <c r="P43" s="1">
+        <v>41505</v>
+      </c>
+      <c r="Q43">
+        <v>100</v>
+      </c>
+      <c r="X43" s="1">
+        <v>41505</v>
+      </c>
+      <c r="Y43">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="8:25">
+      <c r="H44" s="1">
+        <v>41526</v>
+      </c>
+      <c r="I44">
+        <v>100</v>
+      </c>
+      <c r="P44" s="1">
+        <v>41526</v>
+      </c>
+      <c r="Q44">
+        <v>100</v>
+      </c>
+      <c r="X44" s="1">
+        <v>41526</v>
+      </c>
+      <c r="Y44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="8:25">
+      <c r="H45" s="1">
+        <v>41533</v>
+      </c>
+      <c r="I45">
+        <v>100</v>
+      </c>
+      <c r="P45" s="1">
+        <v>41533</v>
+      </c>
+      <c r="Q45">
+        <v>100</v>
+      </c>
+      <c r="X45" s="1">
+        <v>41533</v>
+      </c>
+      <c r="Y45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="8:25">
+      <c r="H46" s="1">
+        <v>41540</v>
+      </c>
+      <c r="I46">
+        <v>100</v>
+      </c>
+      <c r="P46" s="1">
+        <v>41540</v>
+      </c>
+      <c r="Q46">
+        <v>100</v>
+      </c>
+      <c r="X46" s="1">
+        <v>41540</v>
+      </c>
+      <c r="Y46">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="8:25">
+      <c r="H47" s="1">
+        <v>41547</v>
+      </c>
+      <c r="I47">
+        <v>100</v>
+      </c>
+      <c r="P47" s="1">
+        <v>41547</v>
+      </c>
+      <c r="Q47">
+        <v>100</v>
+      </c>
+      <c r="X47" s="1">
+        <v>41547</v>
+      </c>
+      <c r="Y47">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="8:25">
+      <c r="H48" s="1">
+        <v>41554</v>
+      </c>
+      <c r="I48">
+        <v>100</v>
+      </c>
+      <c r="P48" s="1">
+        <v>41554</v>
+      </c>
+      <c r="Q48">
+        <v>100</v>
+      </c>
+      <c r="X48" s="1">
+        <v>41554</v>
+      </c>
+      <c r="Y48">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="8:25">
+      <c r="H49" s="1">
+        <v>41561</v>
+      </c>
+      <c r="I49">
+        <v>100</v>
+      </c>
+      <c r="P49" s="1">
+        <v>41561</v>
+      </c>
+      <c r="Q49">
+        <v>100</v>
+      </c>
+      <c r="X49" s="1">
+        <v>41561</v>
+      </c>
+      <c r="Y49">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="8:25">
+      <c r="H50" s="1">
+        <v>41568</v>
+      </c>
+      <c r="I50">
+        <v>100</v>
+      </c>
+      <c r="P50" s="1">
+        <v>41568</v>
+      </c>
+      <c r="Q50">
+        <v>100</v>
+      </c>
+      <c r="X50" s="1">
+        <v>41568</v>
+      </c>
+      <c r="Y50">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="8:25">
+      <c r="H51" s="1">
+        <v>41575</v>
+      </c>
+      <c r="I51">
+        <v>100</v>
+      </c>
+      <c r="P51" s="1">
+        <v>41575</v>
+      </c>
+      <c r="Q51">
+        <v>100</v>
+      </c>
+      <c r="X51" s="1">
+        <v>41575</v>
+      </c>
+      <c r="Y51">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="8:25">
+      <c r="H52" s="1">
+        <v>41593</v>
+      </c>
+      <c r="I52">
+        <v>200</v>
+      </c>
+      <c r="P52" s="1">
+        <v>41593</v>
+      </c>
+      <c r="Q52">
+        <v>200</v>
+      </c>
+      <c r="X52" s="1">
+        <v>41593</v>
+      </c>
+      <c r="Y52">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" spans="8:25">
+      <c r="H53" s="1">
+        <v>41596</v>
+      </c>
+      <c r="I53">
+        <v>100</v>
+      </c>
+      <c r="P53" s="1">
+        <v>41596</v>
+      </c>
+      <c r="Q53">
+        <v>100</v>
+      </c>
+      <c r="X53" s="1">
+        <v>41596</v>
+      </c>
+      <c r="Y53">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="8:25">
+      <c r="H54" s="1">
+        <v>41603</v>
+      </c>
+      <c r="I54">
+        <v>100</v>
+      </c>
+      <c r="P54" s="1">
+        <v>41603</v>
+      </c>
+      <c r="Q54">
+        <v>100</v>
+      </c>
+      <c r="X54" s="1">
+        <v>41603</v>
+      </c>
+      <c r="Y54">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="8:25">
+      <c r="H55" s="1">
+        <v>41607</v>
+      </c>
+      <c r="I55">
+        <v>100</v>
+      </c>
+      <c r="P55" s="1">
+        <v>41607</v>
+      </c>
+      <c r="Q55">
+        <v>100</v>
+      </c>
+      <c r="X55" s="1">
+        <v>41607</v>
+      </c>
+      <c r="Y55">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="8:25">
+      <c r="H56" s="1">
+        <v>41617</v>
+      </c>
+      <c r="I56">
+        <v>100</v>
+      </c>
+      <c r="P56" s="1">
+        <v>41617</v>
+      </c>
+      <c r="Q56">
+        <v>100</v>
+      </c>
+      <c r="X56" s="1">
+        <v>41617</v>
+      </c>
+      <c r="Y56">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="8:25">
+      <c r="H57" s="1">
+        <v>41624</v>
+      </c>
+      <c r="I57">
+        <v>100</v>
+      </c>
+      <c r="P57" s="1">
+        <v>41624</v>
+      </c>
+      <c r="Q57">
+        <v>100</v>
+      </c>
+      <c r="X57" s="1">
+        <v>41624</v>
+      </c>
+      <c r="Y57">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="8:25">
+      <c r="H58" s="1">
+        <v>41631</v>
+      </c>
+      <c r="I58">
+        <v>100</v>
+      </c>
+      <c r="P58" s="1">
+        <v>41631</v>
+      </c>
+      <c r="Q58">
+        <v>100</v>
+      </c>
+      <c r="X58" s="1">
+        <v>41631</v>
+      </c>
+      <c r="Y58">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="8:25">
+      <c r="H59" s="1">
+        <v>41638</v>
+      </c>
+      <c r="I59">
+        <v>100</v>
+      </c>
+      <c r="P59" s="1">
+        <v>41638</v>
+      </c>
+      <c r="Q59">
+        <v>100</v>
+      </c>
+      <c r="X59" s="1">
+        <v>41638</v>
+      </c>
+      <c r="Y59">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="8:25">
+      <c r="H60" s="1">
+        <v>41639</v>
+      </c>
+      <c r="I60">
+        <v>-14585.1</v>
+      </c>
+      <c r="P60" s="1">
+        <v>41639</v>
+      </c>
+      <c r="Q60">
+        <f>I60-49.95-29.97-29.97-29.97</f>
+        <v>-14724.96</v>
+      </c>
+      <c r="X60" s="1">
+        <v>41639</v>
+      </c>
+      <c r="Y60" s="51">
+        <f>Q60-SUM(K12:Q12)</f>
+        <v>-14430.723099999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="R6:Y6"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="T13:U13"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="X13:Y13"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="J6:Q6"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>